<commit_message>
fixed name_to_properties and its testing
</commit_message>
<xml_diff>
--- a/example/data/classifications_codes_fractions.xlsx
+++ b/example/data/classifications_codes_fractions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/PyGCMS/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cornellprod-my.sharepoint.com/personal/mp933_cornell_edu/Documents/Python/gcms_data_analysis/example/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1676" documentId="11_6A69D6BF87B0D5004BBA281159F860B048AFFA68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FA4CEA0-A5DD-4043-B2DE-254D07DA736F}"/>
+  <xr:revisionPtr revIDLastSave="1677" documentId="11_6A69D6BF87B0D5004BBA281159F860B048AFFA68" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBC9F577-CD28-41E1-B5CB-FCA761BB2F40}"/>
   <bookViews>
-    <workbookView xWindow="14370" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -923,10 +923,6 @@
       <c r="B2" t="s">
         <v>45</v>
       </c>
-      <c r="C2">
-        <f xml:space="preserve"> 12.011*2 + 2*15.999 + 1.008*3</f>
-        <v>59.043999999999997</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">

</xml_diff>